<commit_message>
Average analysis complete, main need to be finish
</commit_message>
<xml_diff>
--- a/Results_ZC/Average_results_Demand_5.xlsx
+++ b/Results_ZC/Average_results_Demand_5.xlsx
@@ -12,6 +12,7 @@
     <sheet name="FTNC_Average_Demand52" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="FTNC_Average_Demand53" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="FTNC_Average_Demand54" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="FTHC_Average_Demand5" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -761,4 +762,72 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Tardiness</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>FTHC_Average_Demand_5</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>12.11441948061514</v>
+      </c>
+      <c r="C2" t="n">
+        <v>182.7178957992942</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>7.255286811132406</v>
+      </c>
+      <c r="F2" t="n">
+        <v>202.0876020910418</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
graphic modified, long time for executing
</commit_message>
<xml_diff>
--- a/Results_ZC/Average_results_Demand_5.xlsx
+++ b/Results_ZC/Average_results_Demand_5.xlsx
@@ -13,6 +13,7 @@
     <sheet name="FTNC_Average_Demand53" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="FTNC_Average_Demand54" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="FTHC_Average_Demand5" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="FTNC_Average_Demand55" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -830,4 +831,72 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Tardiness</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>FTNC_Average_Demand_5</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2323.045558379758</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12927.3257339221</v>
+      </c>
+      <c r="D2" t="n">
+        <v>515.0616311181449</v>
+      </c>
+      <c r="E2" t="n">
+        <v>64.17206500977974</v>
+      </c>
+      <c r="F2" t="n">
+        <v>15829.60498842978</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>